<commit_message>
Revised all country data
</commit_message>
<xml_diff>
--- a/src/Data/country_data.xlsx
+++ b/src/Data/country_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\OneDrive\Documents\mr-risk-assessment\src\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5aee5c5b004427f/Documents/mr-risk-assessment/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB21942-1E30-4A3E-86F4-D1438ED0EF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4BB21942-1E30-4A3E-86F4-D1438ED0EF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD21880B-75E8-4AF5-B322-9F16D1725E49}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="773" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="229">
   <si>
     <t>Case ID</t>
   </si>
@@ -1068,9 +1068,6 @@
     <t>Cobertura de la última campaña de seguimiento</t>
   </si>
   <si>
-    <t>Porcentaje de hospitales de nivel subnacional con personal capacitado para hacer triaje y aislar casos altamente sospechosos de sarampión y rubéola</t>
-  </si>
-  <si>
     <t>BELIZE</t>
   </si>
   <si>
@@ -1099,6 +1096,9 @@
   </si>
   <si>
     <t>Presencia de un equipo subnacional de respuesta rápida capacitado a nivel subnacional (Si/No)</t>
+  </si>
+  <si>
+    <t>El equipo subnacional de respuesta rápida fue entrenado en los últimos 2 años</t>
   </si>
 </sst>
 </file>
@@ -3136,7 +3136,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+    <sheetView zoomScale="139" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3160,7 +3160,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3213,10 +3213,10 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3278,10 +3278,10 @@
         <v>90</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E2" s="51">
         <v>120600</v>
@@ -3298,10 +3298,10 @@
         <v>91</v>
       </c>
       <c r="C3" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>219</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>220</v>
       </c>
       <c r="E3" s="52">
         <v>96197</v>
@@ -3318,10 +3318,10 @@
         <v>93</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" s="52">
         <v>48429</v>
@@ -3338,10 +3338,10 @@
         <v>95</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E5" s="52">
         <v>51749</v>
@@ -3358,10 +3358,10 @@
         <v>97</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E6" s="52">
         <v>43944</v>
@@ -3378,10 +3378,10 @@
         <v>99</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E7" s="52">
         <v>37614</v>
@@ -3511,10 +3511,10 @@
         <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E3" s="31">
         <v>97</v>
@@ -3558,10 +3558,10 @@
         <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="E4" s="31">
         <v>94</v>
@@ -3605,10 +3605,10 @@
         <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="31">
         <v>95</v>
@@ -3652,10 +3652,10 @@
         <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" s="31">
         <v>96</v>
@@ -3699,10 +3699,10 @@
         <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E7" s="31">
         <v>94</v>
@@ -3746,10 +3746,10 @@
         <v>99</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E8" s="31">
         <v>96</v>
@@ -3889,10 +3889,10 @@
         <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E3" s="31">
         <v>1839</v>
@@ -3920,10 +3920,10 @@
         <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="E4" s="31">
         <v>1636</v>
@@ -3951,10 +3951,10 @@
         <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="31">
         <v>717</v>
@@ -3982,10 +3982,10 @@
         <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" s="31">
         <v>1025</v>
@@ -4013,10 +4013,10 @@
         <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E7" s="31">
         <v>979</v>
@@ -4044,10 +4044,10 @@
         <v>99</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E8" s="31">
         <v>597</v>
@@ -4190,10 +4190,10 @@
         <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E3" s="31" t="s">
         <v>41</v>
@@ -4228,10 +4228,10 @@
         <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="E4" s="31" t="s">
         <v>41</v>
@@ -4266,10 +4266,10 @@
         <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>41</v>
@@ -4304,10 +4304,10 @@
         <v>95</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>41</v>
@@ -4342,10 +4342,10 @@
         <v>97</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>41</v>
@@ -4380,10 +4380,10 @@
         <v>99</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E8" s="31" t="s">
         <v>41</v>
@@ -4869,7 +4869,7 @@
         <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>88</v>
@@ -4926,7 +4926,7 @@
         <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>92</v>
@@ -4983,7 +4983,7 @@
         <v>90</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>88</v>
@@ -5040,7 +5040,7 @@
         <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>88</v>
@@ -5097,7 +5097,7 @@
         <v>91</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>92</v>
@@ -5156,7 +5156,7 @@
         <v>91</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>92</v>
@@ -5215,7 +5215,7 @@
         <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>92</v>
@@ -5272,7 +5272,7 @@
         <v>97</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>98</v>
@@ -5329,7 +5329,7 @@
         <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>92</v>
@@ -5388,7 +5388,7 @@
         <v>91</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>92</v>
@@ -5445,7 +5445,7 @@
         <v>93</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>94</v>
@@ -5502,7 +5502,7 @@
         <v>93</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>94</v>
@@ -5561,7 +5561,7 @@
         <v>91</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>92</v>
@@ -5620,7 +5620,7 @@
         <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>92</v>
@@ -5677,7 +5677,7 @@
         <v>99</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>100</v>
@@ -5734,7 +5734,7 @@
         <v>97</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>98</v>
@@ -5793,7 +5793,7 @@
         <v>97</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>98</v>
@@ -5850,7 +5850,7 @@
         <v>99</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>100</v>
@@ -5907,7 +5907,7 @@
         <v>91</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>92</v>
@@ -5966,7 +5966,7 @@
         <v>91</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>92</v>
@@ -6023,7 +6023,7 @@
         <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>94</v>
@@ -6080,7 +6080,7 @@
         <v>97</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>98</v>
@@ -6139,7 +6139,7 @@
         <v>99</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>100</v>
@@ -6198,7 +6198,7 @@
         <v>99</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>100</v>
@@ -6257,7 +6257,7 @@
         <v>97</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>98</v>
@@ -6316,7 +6316,7 @@
         <v>90</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>88</v>
@@ -6373,7 +6373,7 @@
         <v>97</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>98</v>
@@ -6430,7 +6430,7 @@
         <v>99</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>100</v>
@@ -6487,7 +6487,7 @@
         <v>99</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>100</v>
@@ -6546,7 +6546,7 @@
         <v>99</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>100</v>
@@ -6605,7 +6605,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D44" s="19" t="s">
         <v>96</v>
@@ -6662,7 +6662,7 @@
         <v>99</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D45" s="19" t="s">
         <v>100</v>
@@ -6719,7 +6719,7 @@
         <v>91</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D46" s="19" t="s">
         <v>92</v>
@@ -6778,7 +6778,7 @@
         <v>97</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>98</v>
@@ -6837,7 +6837,7 @@
         <v>97</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D48" s="19" t="s">
         <v>98</v>
@@ -6896,7 +6896,7 @@
         <v>97</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>98</v>
@@ -6953,7 +6953,7 @@
         <v>90</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>88</v>
@@ -7010,7 +7010,7 @@
         <v>90</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D51" s="56" t="s">
         <v>88</v>
@@ -7069,7 +7069,7 @@
         <v>90</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D52" s="56" t="s">
         <v>88</v>
@@ -7128,7 +7128,7 @@
         <v>97</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D53" s="19" t="s">
         <v>98</v>
@@ -7185,7 +7185,7 @@
         <v>90</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D54" s="56" t="s">
         <v>88</v>
@@ -7242,7 +7242,7 @@
         <v>99</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D55" s="19" t="s">
         <v>100</v>
@@ -7301,7 +7301,7 @@
         <v>97</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>98</v>
@@ -7360,7 +7360,7 @@
         <v>99</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D57" s="19" t="s">
         <v>100</v>
@@ -7419,7 +7419,7 @@
         <v>93</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D58" s="19" t="s">
         <v>94</v>
@@ -7478,7 +7478,7 @@
         <v>99</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D59" s="19" t="s">
         <v>100</v>
@@ -7535,7 +7535,7 @@
         <v>93</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D60" s="19" t="s">
         <v>94</v>
@@ -7594,7 +7594,7 @@
         <v>99</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D61" s="19" t="s">
         <v>100</v>
@@ -7651,7 +7651,7 @@
         <v>91</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>92</v>
@@ -7710,7 +7710,7 @@
         <v>90</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D63" s="19" t="s">
         <v>88</v>
@@ -7767,7 +7767,7 @@
         <v>90</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D64" s="19" t="s">
         <v>88</v>
@@ -7824,7 +7824,7 @@
         <v>93</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D65" s="19" t="s">
         <v>94</v>
@@ -7883,7 +7883,7 @@
         <v>91</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D66" s="19" t="s">
         <v>92</v>
@@ -7942,7 +7942,7 @@
         <v>90</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D67" s="19" t="s">
         <v>88</v>
@@ -8001,7 +8001,7 @@
         <v>99</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D68" s="19" t="s">
         <v>100</v>
@@ -8060,7 +8060,7 @@
         <v>91</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D69" s="19" t="s">
         <v>92</v>
@@ -8119,7 +8119,7 @@
         <v>90</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D70" s="19" t="s">
         <v>88</v>
@@ -8176,7 +8176,7 @@
         <v>90</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D71" s="19" t="s">
         <v>88</v>
@@ -8837,8 +8837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -8865,10 +8865,10 @@
         <v>31</v>
       </c>
       <c r="E1" s="39" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" s="39" t="s">
         <v>228</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -8879,16 +8879,16 @@
         <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="30">
-        <v>50</v>
+      <c r="F2" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -8899,16 +8899,16 @@
         <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="E3" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="30">
-        <v>50</v>
+      <c r="F3" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -8919,16 +8919,16 @@
         <v>93</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="30">
-        <v>50</v>
+      <c r="F4" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -8939,16 +8939,16 @@
         <v>95</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="30">
-        <v>50</v>
+      <c r="F5" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8959,16 +8959,16 @@
         <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="30">
-        <v>50</v>
+      <c r="F6" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
@@ -8979,16 +8979,16 @@
         <v>99</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="30">
-        <v>50</v>
+      <c r="F7" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -9138,6 +9138,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007C69FE739999C447A76F1EF8B3FD66E4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cbd048430c8551c34c2c3c8571f1b260">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4655c133-e14e-4d88-8fbc-c3b347145ec5" xmlns:ns4="64ced670-a384-4657-ba0f-fc07d30f5a44" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5457dbb80d17598a17de4d439e456cf2" ns3:_="" ns4:_="">
     <xsd:import namespace="4655c133-e14e-4d88-8fbc-c3b347145ec5"/>
@@ -9360,36 +9375,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1C9E008-75C3-4280-8CCC-7498B59407BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6264E33-6917-4678-8EC8-8D88A2F9795C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4655c133-e14e-4d88-8fbc-c3b347145ec5"/>
-    <ds:schemaRef ds:uri="64ced670-a384-4657-ba0f-fc07d30f5a44"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9412,9 +9401,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6264E33-6917-4678-8EC8-8D88A2F9795C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1C9E008-75C3-4280-8CCC-7498B59407BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4655c133-e14e-4d88-8fbc-c3b347145ec5"/>
+    <ds:schemaRef ds:uri="64ced670-a384-4657-ba0f-fc07d30f5a44"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modified rapid response to include the trained personeel in the last 2 years question
</commit_message>
<xml_diff>
--- a/src/Data/country_data.xlsx
+++ b/src/Data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5aee5c5b004427f/Documents/mr-risk-assessment/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4BB21942-1E30-4A3E-86F4-D1438ED0EF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD21880B-75E8-4AF5-B322-9F16D1725E49}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{4BB21942-1E30-4A3E-86F4-D1438ED0EF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8953C81A-259F-4307-8A2A-661895AAA372}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="773" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="229">
   <si>
     <t>Case ID</t>
   </si>
@@ -1092,13 +1092,13 @@
     <t>Belize</t>
   </si>
   <si>
-    <t>SPA</t>
-  </si>
-  <si>
     <t>Presencia de un equipo subnacional de respuesta rápida capacitado a nivel subnacional (Si/No)</t>
   </si>
   <si>
     <t>El equipo subnacional de respuesta rápida fue entrenado en los últimos 2 años</t>
+  </si>
+  <si>
+    <t>ENG</t>
   </si>
 </sst>
 </file>
@@ -2067,7 +2067,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="d/mm/yy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2096,7 +2096,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="d/mm/yy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2125,7 +2125,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="d/mm/yy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2153,7 +2153,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="d/mm/yy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2181,7 +2181,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="d/mm/yy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -2262,7 +2262,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="d/mm/yy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -3136,8 +3136,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="139" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3208,7 +3208,7 @@
         <v>87</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3216,7 +3216,7 @@
         <v>224</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4431,8 +4431,8 @@
   </sheetPr>
   <dimension ref="A1:S112"/>
   <sheetViews>
-    <sheetView topLeftCell="G8" zoomScale="109" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView topLeftCell="B56" zoomScale="109" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -8128,7 +8128,7 @@
         <v>209</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G70" s="21">
         <v>43217</v>
@@ -8837,8 +8837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -8865,10 +8865,10 @@
         <v>31</v>
       </c>
       <c r="E1" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="39" t="s">
         <v>227</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -8885,7 +8885,7 @@
         <v>218</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>41</v>
@@ -8908,7 +8908,7 @@
         <v>41</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -8925,10 +8925,10 @@
         <v>220</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -8944,11 +8944,9 @@
       <c r="D5" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>41</v>
-      </c>
+      <c r="E5" s="30"/>
       <c r="F5" s="30" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8967,9 +8965,7 @@
       <c r="E6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="30" t="s">
-        <v>41</v>
-      </c>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="44" t="s">
@@ -8993,6 +8989,11 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F7" xr:uid="{2D944F37-CA13-42B4-BF24-9DD447030077}">
+      <formula1>"Si,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9138,18 +9139,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9376,14 +9377,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6264E33-6917-4678-8EC8-8D88A2F9795C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A51E5E2-41F2-4A1F-A4B0-950DEDB4B143}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -9396,6 +9389,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6264E33-6917-4678-8EC8-8D88A2F9795C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fixed QA report error with outbreak
</commit_message>
<xml_diff>
--- a/src/Data/country_data.xlsx
+++ b/src/Data/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5aee5c5b004427f/Documents/mr-risk-assessment/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{4BB21942-1E30-4A3E-86F4-D1438ED0EF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8953C81A-259F-4307-8A2A-661895AAA372}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{4BB21942-1E30-4A3E-86F4-D1438ED0EF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A564E2A-06D1-4D86-9D81-7ADF759645F3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -1098,7 +1098,7 @@
     <t>El equipo subnacional de respuesta rápida fue entrenado en los últimos 2 años</t>
   </si>
   <si>
-    <t>ENG</t>
+    <t>SPA</t>
   </si>
 </sst>
 </file>
@@ -3137,7 +3137,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>

</xml_diff>